<commit_message>
includes parsing for test file
</commit_message>
<xml_diff>
--- a/samplefile.xlsx
+++ b/samplefile.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bebre\PycharmProjects\FileIntegrity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61D4003D-4345-4E9F-83ED-124F0AE834FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D9CA909-9CEA-4149-AED1-92C262173435}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11265" xr2:uid="{B21373EB-6263-43E7-8D7B-AB9475E6D518}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="16920" windowHeight="10540" xr2:uid="{B21373EB-6263-43E7-8D7B-AB9475E6D518}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="samplefile" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>isWeekday</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>custom5</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -95,8 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,686 +415,752 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F93F9D4-8F3A-45F9-9BD6-EDCEA81C2E5D}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I9:I14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>43606</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>10000</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>5000</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>-1</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.5</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>43607</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>10000</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5005</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.2</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>-0.5</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.6</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>43608</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>15000</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5100</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>-0.6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.8</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
+      <c r="K4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>43609</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>-1</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>10100</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>5135</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>-1.4</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.5</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.8</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>43610</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>12600</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>5185</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1.6</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>0.9</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>43611</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>13130</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>5235</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>-3</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.5</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>43612</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>13660</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>5285</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>-3.8</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2.4</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>43613</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>10000</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5335</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2.8</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>2.5</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>43614</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>10000</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>5385</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>-5.4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3.2</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>3</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1.3</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1.9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>43615</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>15000</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>5435</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>-6.2</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>3.6</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>3.5</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1.4</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2.1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>43616</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>10100</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>5485</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>-7</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
       </c>
       <c r="H12">
         <v>4</v>
       </c>
       <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
         <v>1.5</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>43617</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>12600</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>5535</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>-7.8</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>4.5</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1.6</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>43618</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>13130</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>5585</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-8.6</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>4.8</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>5</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1.7</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>2.7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>43619</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>10000</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>5635</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>-9.4</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>5.2</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>5.5</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1.8</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>2.9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>43620</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>10000</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>5685</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>-10.199999999999999</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>5.6</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>6</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1.9</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>3.1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>43621</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>15000</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>5735</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>-11</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>6</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>6.5</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>2</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>3.3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>43622</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>10100</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>5785</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>-11.8</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>6.4</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>7</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>2.1</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>3.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>43623</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
         <v>12600</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>5835</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>-12.6</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>6.8</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>7.5</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>3.7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>43624</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>13130</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>5885</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>-13.4</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>7.2</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>8</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>3.9</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>43625</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>13660</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>5935</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>-14.2</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>7.6</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>8.5</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>2.4</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>4.0999999999999996</v>
       </c>
     </row>

</xml_diff>